<commit_message>
this is new branch
</commit_message>
<xml_diff>
--- a/bin/testcase/Leads.xlsx
+++ b/bin/testcase/Leads.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="64">
   <si>
     <t>TCID</t>
   </si>
@@ -560,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,6 +1047,26 @@
       </c>
       <c r="F24" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>